<commit_message>
New Mall location file
</commit_message>
<xml_diff>
--- a/media/LocationsExcels/mall_location.xlsx
+++ b/media/LocationsExcels/mall_location.xlsx
@@ -13,7 +13,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>branch_name</t>
+    <t>mall_name</t>
   </si>
   <si>
     <t>telephone_number</t>
@@ -67,9 +67,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
@@ -107,16 +110,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>